<commit_message>
latest version cohort (removed totals at the last row, generating missing values)
</commit_message>
<xml_diff>
--- a/data/realpop.xlsx
+++ b/data/realpop.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\md21\Dropbox\UBx\TB-SPEED\Modelling\O3SAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\md21\Dropbox\UBx\TB-SPEED\Modelling\O3SAM\TBSsam\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2621BB-3E87-4B0B-86C0-04F60D007768}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF495C-488F-40A4-AF2A-A46AD77836CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2136,12 +2136,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2498,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ436"/>
+  <dimension ref="A1:CJ435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="BK2" sqref="BK2"/>
+    <sheetView tabSelected="1" topLeftCell="A427" workbookViewId="0">
+      <selection activeCell="AP438" sqref="AP438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,25 +2650,25 @@
       <c r="AT1" t="s">
         <v>535</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AU1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AV1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AX1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AY1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="4" t="s">
         <v>537</v>
       </c>
       <c r="BB1" t="s">
@@ -99917,7 +99916,7 @@
         <v>0</v>
       </c>
       <c r="BA387">
-        <f t="shared" ref="BA387:BA436" si="6">SUM(AU387:AZ387)</f>
+        <f t="shared" ref="BA387:BA435" si="6">SUM(AU387:AZ387)</f>
         <v>0</v>
       </c>
       <c r="BB387">
@@ -111406,20 +111405,6 @@
       </c>
       <c r="CJ435" s="1">
         <v>5</v>
-      </c>
-    </row>
-    <row r="436" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="BK436" s="4">
-        <f>COUNTIF(BK2:BK435,"&lt;10")</f>
-        <v>351</v>
-      </c>
-      <c r="BV436" s="4">
-        <f>COUNTIF(BV2:BV435,"&lt;10")</f>
-        <v>151</v>
-      </c>
-      <c r="CJ436" s="4">
-        <f>COUNTIF(CJ2:CJ435,"&lt;10")+COUNTIF(CJ2:CJ435,"")</f>
-        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>